<commit_message>
Updating combined data and headshots file along with code
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\Baseball\Player Listing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0994002B-E0EB-4EF4-8626-1B9A6BB3D420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D5F90-7322-461E-B9DF-390E549BC9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="327">
   <si>
     <t>Name</t>
   </si>
@@ -1076,12 +1076,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1419,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1736,6 +1735,9 @@
       <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C31" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -3019,7 +3021,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="4" t="s">
+      <c r="A164" t="s">
         <v>324</v>
       </c>
       <c r="B164" s="2" t="s">

</xml_diff>

<commit_message>
Updating Daily stats and code for 3 name pitchers
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F990C4-D093-4A0A-B60F-98083EC84444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A2B61-538A-4A08-84E2-39A3BBE11E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="359">
   <si>
     <t>Name</t>
   </si>
@@ -1086,6 +1086,36 @@
   </si>
   <si>
     <t>https://midfield.mlbstatic.com/v1/people/683627/spots/120</t>
+  </si>
+  <si>
+    <t>Dane Dunning</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/641540/spots/120</t>
+  </si>
+  <si>
+    <t>Andre Pallante</t>
+  </si>
+  <si>
+    <t>Keider Montero</t>
+  </si>
+  <si>
+    <t>Spencer Schwellenbach</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/669467/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/672456/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/680885/spots/120</t>
+  </si>
+  <si>
+    <t>David Peterson</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/656849/spots/120</t>
   </si>
 </sst>
 </file>
@@ -1475,16 +1505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B169" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="133" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -3375,6 +3405,9 @@
       <c r="B172" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="C172" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
@@ -3383,6 +3416,9 @@
       <c r="B173" s="2" t="s">
         <v>345</v>
       </c>
+      <c r="C173" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
@@ -3391,6 +3427,9 @@
       <c r="B174" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="C174" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
@@ -3399,6 +3438,9 @@
       <c r="B175" s="2" t="s">
         <v>347</v>
       </c>
+      <c r="C175" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
@@ -3406,6 +3448,61 @@
       </c>
       <c r="B176" s="2" t="s">
         <v>348</v>
+      </c>
+      <c r="C176" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>349</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C177" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>351</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C178" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>352</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C179" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>353</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C180" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>357</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3593,6 +3690,11 @@
     <hyperlink ref="B174" r:id="rId176" xr:uid="{063DB121-1B09-4C4A-A7CB-67F92A70E822}"/>
     <hyperlink ref="B175" r:id="rId177" xr:uid="{4529126A-013E-48BE-BF9C-0857DD382C6C}"/>
     <hyperlink ref="B176" r:id="rId178" xr:uid="{2F41BBD7-2015-4D42-8F88-8932B17FA34E}"/>
+    <hyperlink ref="B177" r:id="rId179" xr:uid="{E3EEE818-F47C-4DA4-97C5-449CA4C17CE4}"/>
+    <hyperlink ref="B178" r:id="rId180" xr:uid="{9F68A673-C7E6-4A90-BBDE-1C7409208E96}"/>
+    <hyperlink ref="B179" r:id="rId181" xr:uid="{889380E0-647D-4489-BE9B-25BAE5EB7861}"/>
+    <hyperlink ref="B180" r:id="rId182" xr:uid="{E541544B-61E3-4737-BBE7-E7662EC00A72}"/>
+    <hyperlink ref="B181" r:id="rId183" xr:uid="{4BE71305-E922-40EC-A901-A899B6397770}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating with tabs and new files
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27877CA8-09D7-4BB7-A2CA-98FDE12DEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76048424-1465-4DCD-BBBC-D82464CB7671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="393">
   <si>
     <t>Name</t>
   </si>
@@ -1200,6 +1200,24 @@
   </si>
   <si>
     <t>https://midfield.mlbstatic.com/v1/people/663687/spots/120</t>
+  </si>
+  <si>
+    <t>Gavin Stone</t>
+  </si>
+  <si>
+    <t>Luis Medina</t>
+  </si>
+  <si>
+    <t>Luis Ortiz</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/665622/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/694813/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/123456/spots/120</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3744,6 +3762,36 @@
       </c>
       <c r="C195" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>387</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C196" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>388</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C197" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>389</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3950,6 +3998,9 @@
     <hyperlink ref="B193" r:id="rId195" xr:uid="{075C6DD4-9B5F-454C-9441-F8AB51EBBED6}"/>
     <hyperlink ref="B194" r:id="rId196" xr:uid="{2AB02CE7-6DE6-4936-A9B6-C3A30517DB7F}"/>
     <hyperlink ref="B195" r:id="rId197" xr:uid="{3FA450BF-3E01-439C-8C3C-97285CDF42E4}"/>
+    <hyperlink ref="B196" r:id="rId198" xr:uid="{B7C88999-8CA0-468E-9DB7-0C84FECCE62D}"/>
+    <hyperlink ref="B197" r:id="rId199" xr:uid="{4030FD80-AC58-4604-AAD9-3C8DDF33D9BF}"/>
+    <hyperlink ref="B198" r:id="rId200" xr:uid="{A6D3B7B5-05D6-404A-A466-9DFEDA40D0C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing pitcher name issue
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1137630-64C4-4A64-B806-97D34D6D4FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79695CCE-603F-48A7-90F8-4C9E2FD32370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="401">
   <si>
     <t>Name</t>
   </si>
@@ -1236,6 +1236,12 @@
   </si>
   <si>
     <t>Carlos Rodón</t>
+  </si>
+  <si>
+    <t>Carlos Rodon</t>
+  </si>
+  <si>
+    <t>Baseball_Savant_Name</t>
   </si>
 </sst>
 </file>
@@ -1625,2439 +1631,3043 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>311</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>255</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>253</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>225</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>313</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>286</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>249</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>265</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>261</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>251</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>270</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>399</v>
+      </c>
+      <c r="B25" t="s">
         <v>398</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>227</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>229</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>289</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>155</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C36" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C37" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>272</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C38" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>206</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>206</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>201</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C44" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C45" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>208</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C46" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>231</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>178</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C48" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C49" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>291</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
+        <v>291</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C51" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C52" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C54" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C55" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C56" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C57" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>141</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C58" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>280</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C59" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C60" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>293</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C61" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>257</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" t="s">
+        <v>257</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C62" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C63" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C64" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C65" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>48</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C66" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>110</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C67" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>275</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" t="s">
+        <v>275</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C68" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C69" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>59</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C70" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C71" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>205</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C72" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>31</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C73" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C74" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>322</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" t="s">
+        <v>322</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>323</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" t="s">
+        <v>323</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C76" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>301</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" t="s">
+        <v>301</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C77" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>149</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C78" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>17</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C79" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C80" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>18</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C81" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>306</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" t="s">
+        <v>306</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C82" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>28</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C83" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>160</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C84" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>198</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C85" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>263</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C86" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>233</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" t="s">
+        <v>233</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C87" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>295</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" t="s">
+        <v>295</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C88" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" t="s">
+        <v>174</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C89" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" t="s">
+        <v>209</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C90" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>135</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C91" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>151</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" t="s">
+        <v>151</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C92" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>19</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C93" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" t="s">
+        <v>96</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C94" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>90</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C95" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C96" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>324</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" t="s">
+        <v>324</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C97" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>139</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" t="s">
+        <v>139</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C98" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>284</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C99" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>127</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" t="s">
+        <v>127</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C100" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>114</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" t="s">
+        <v>114</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C101" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>131</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" t="s">
+        <v>131</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C102" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" t="s">
+        <v>235</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C103" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>297</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" t="s">
+        <v>297</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C104" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>184</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C105" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>78</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" t="s">
+        <v>78</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C106" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>308</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" t="s">
+        <v>308</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C107" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>20</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C108" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>144</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" t="s">
+        <v>144</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C109" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>304</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" t="s">
+        <v>304</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C110" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>325</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" t="s">
+        <v>325</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C111" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>125</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" t="s">
+        <v>125</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C112" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>274</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" t="s">
+        <v>274</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C113" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>299</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" t="s">
+        <v>299</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C114" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>210</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" t="s">
+        <v>210</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C115" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>64</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C116" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>21</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C117" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>237</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" t="s">
+        <v>237</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C118" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>282</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C119" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>32</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" t="s">
+        <v>32</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C120" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>192</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" t="s">
+        <v>192</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C121" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>239</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" t="s">
+        <v>239</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C122" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>70</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" t="s">
+        <v>70</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C123" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>211</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" t="s">
+        <v>211</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C124" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>190</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" t="s">
+        <v>190</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C125" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>259</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" t="s">
+        <v>259</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C126" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>35</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C127" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>212</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" t="s">
+        <v>212</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C128" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>22</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" t="s">
+        <v>22</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C129" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>310</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" t="s">
+        <v>310</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C130" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>98</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" t="s">
+        <v>98</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C131" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>88</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" t="s">
+        <v>88</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C132" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>129</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" t="s">
+        <v>129</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C133" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>159</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" t="s">
+        <v>159</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C134" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>23</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C135" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>33</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" t="s">
+        <v>33</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C136" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>153</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" t="s">
+        <v>153</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C137" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>326</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" t="s">
+        <v>326</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C138" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>215</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" t="s">
+        <v>215</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C139" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>213</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" t="s">
+        <v>213</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C140" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>302</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" t="s">
+        <v>302</v>
+      </c>
+      <c r="C141" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C141" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>137</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" t="s">
+        <v>137</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C142" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>247</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" t="s">
+        <v>247</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C143" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>75</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" t="s">
+        <v>75</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C144" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>241</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" t="s">
+        <v>241</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C145" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>81</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" t="s">
+        <v>81</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C146" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>214</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" t="s">
+        <v>214</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C147" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>243</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" t="s">
+        <v>243</v>
+      </c>
+      <c r="C148" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C148" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>24</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C149" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>25</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C150" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>268</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" t="s">
+        <v>268</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C151" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>266</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" t="s">
+        <v>266</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C152" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>143</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" t="s">
+        <v>143</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C153" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>245</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B154" t="s">
+        <v>245</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C154" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>167</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" t="s">
+        <v>167</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C155" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>34</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" t="s">
+        <v>34</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C156" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>147</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" t="s">
+        <v>147</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C157" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>327</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" t="s">
+        <v>327</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C158" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>176</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" t="s">
+        <v>176</v>
+      </c>
+      <c r="C159" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C159" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>26</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" t="s">
+        <v>26</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C160" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>273</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" t="s">
+        <v>273</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C161" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>27</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" t="s">
+        <v>27</v>
+      </c>
+      <c r="C162" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C162" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>315</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" t="s">
+        <v>315</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C163" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>317</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" t="s">
+        <v>317</v>
+      </c>
+      <c r="C164" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C164" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>268</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" t="s">
+        <v>268</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C165" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>318</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B166" t="s">
+        <v>318</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C166" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D166" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>328</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" t="s">
+        <v>328</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C167" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D167" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>329</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B168" t="s">
+        <v>329</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C168" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>330</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" t="s">
+        <v>330</v>
+      </c>
+      <c r="C169" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C169" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D169" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>331</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" t="s">
+        <v>331</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C170" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>332</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" t="s">
+        <v>332</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C171" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D171" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>338</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" t="s">
+        <v>338</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C172" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D172" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>339</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" t="s">
+        <v>339</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C173" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D173" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>340</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" t="s">
+        <v>340</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C174" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>341</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" t="s">
+        <v>341</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C175" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>342</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" t="s">
+        <v>342</v>
+      </c>
+      <c r="C176" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C176" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D176" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>348</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B177" t="s">
+        <v>348</v>
+      </c>
+      <c r="C177" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C177" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D177" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>350</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" t="s">
+        <v>350</v>
+      </c>
+      <c r="C178" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C178" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D178" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>351</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" t="s">
+        <v>351</v>
+      </c>
+      <c r="C179" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C179" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D179" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>352</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" t="s">
+        <v>352</v>
+      </c>
+      <c r="C180" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C180" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D180" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>356</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" t="s">
+        <v>356</v>
+      </c>
+      <c r="C181" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C181" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D181" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>358</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" t="s">
+        <v>358</v>
+      </c>
+      <c r="C182" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C182" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D182" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>359</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" t="s">
+        <v>359</v>
+      </c>
+      <c r="C183" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C183" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D183" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>362</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
+        <v>362</v>
+      </c>
+      <c r="C184" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C184" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D184" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>364</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" t="s">
+        <v>364</v>
+      </c>
+      <c r="C185" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C185" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D185" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>366</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" t="s">
+        <v>366</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C186" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D186" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>367</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" t="s">
+        <v>367</v>
+      </c>
+      <c r="C187" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C187" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D187" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>370</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" t="s">
+        <v>370</v>
+      </c>
+      <c r="C188" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C188" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D188" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>371</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" t="s">
+        <v>371</v>
+      </c>
+      <c r="C189" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C189" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D189" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>372</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" t="s">
+        <v>372</v>
+      </c>
+      <c r="C190" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="C190" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D190" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>373</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" t="s">
+        <v>373</v>
+      </c>
+      <c r="C191" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C191" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D191" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>378</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" t="s">
+        <v>378</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="C192" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D192" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>380</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" t="s">
+        <v>380</v>
+      </c>
+      <c r="C193" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C193" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D193" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>381</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B194" t="s">
+        <v>381</v>
+      </c>
+      <c r="C194" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C194" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D194" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>384</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B195" t="s">
+        <v>384</v>
+      </c>
+      <c r="C195" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="C195" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D195" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>386</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B196" t="s">
+        <v>386</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="C196" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D196" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>387</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B197" t="s">
+        <v>387</v>
+      </c>
+      <c r="C197" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C197" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D197" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>393</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B198" t="s">
+        <v>393</v>
+      </c>
+      <c r="C198" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C198" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D198" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>390</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B199" t="s">
+        <v>390</v>
+      </c>
+      <c r="C199" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C199" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D199" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>394</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B200" t="s">
+        <v>394</v>
+      </c>
+      <c r="C200" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C200" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D200" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>395</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B201" t="s">
+        <v>395</v>
+      </c>
+      <c r="C201" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C162">
+  <autoFilter ref="A1:D1" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D162">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B135" r:id="rId1" xr:uid="{C45472D7-1E29-4980-95E0-15D6D01B36FA}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{1EA6B6DE-C528-4BBF-8958-B9D1378CBBEA}"/>
-    <hyperlink ref="B12" r:id="rId3" xr:uid="{4F9BBF32-0E85-44F1-BAE2-FDFE1B91203C}"/>
-    <hyperlink ref="B28" r:id="rId4" xr:uid="{1743C8BA-2A45-4EF9-8EAE-003FA5622677}"/>
-    <hyperlink ref="B120" r:id="rId5" xr:uid="{759148E7-8E0F-41F6-B9F3-BB34C434E2D7}"/>
-    <hyperlink ref="B129" r:id="rId6" xr:uid="{8850343C-EAF0-4713-9C66-21BF05B290EC}"/>
-    <hyperlink ref="B31" r:id="rId7" xr:uid="{CA8DDB4C-49CE-4AA5-B564-1108A8088B23}"/>
-    <hyperlink ref="B45" r:id="rId8" xr:uid="{A96A63DD-6ED4-47E6-B759-BD9FCFC58B60}"/>
-    <hyperlink ref="B162" r:id="rId9" xr:uid="{55C307B9-C21E-4227-B6BA-602B4CDD2E63}"/>
-    <hyperlink ref="B117" r:id="rId10" xr:uid="{FBC71765-97DF-4951-8AED-C771FFA6C3B6}"/>
-    <hyperlink ref="B52" r:id="rId11" xr:uid="{44C0BA97-BC98-4009-9EF5-8C29C471CC2B}"/>
-    <hyperlink ref="B65" r:id="rId12" xr:uid="{83CC39A1-58DF-4F8E-80EF-7133BFDA09E5}"/>
-    <hyperlink ref="B66" r:id="rId13" xr:uid="{A9F4C6E5-7612-40C3-92FF-2F0A1197F32E}"/>
-    <hyperlink ref="B55" r:id="rId14" xr:uid="{29AD0F25-0604-4645-86CB-591ACB87642C}"/>
-    <hyperlink ref="B33" r:id="rId15" xr:uid="{03239B77-EAD5-4377-8E99-41BDC8C35FAF}"/>
-    <hyperlink ref="B57" r:id="rId16" xr:uid="{A963AD17-9953-4B76-B014-99AE04AFBC22}"/>
-    <hyperlink ref="B23" r:id="rId17" xr:uid="{254FC5D9-2139-49F1-AF42-C37C7AD52CF9}"/>
-    <hyperlink ref="B97" r:id="rId18" xr:uid="{ADEC84CE-4B4C-475A-B45C-A5A25ABA57F9}"/>
-    <hyperlink ref="B70" r:id="rId19" xr:uid="{A903E050-8C42-4183-880A-565DF6E20245}"/>
-    <hyperlink ref="B3" r:id="rId20" xr:uid="{E83EAE86-523E-449E-8625-E0FCBC6EDE67}"/>
-    <hyperlink ref="B158" r:id="rId21" xr:uid="{4F43B789-DA90-4D7B-B4C4-7719C98AFEF4}"/>
-    <hyperlink ref="B116" r:id="rId22" xr:uid="{1073D5D0-0D5E-4AB1-940D-24EDB5EF0E1D}"/>
-    <hyperlink ref="B74" r:id="rId23" xr:uid="{30F225A0-9236-482B-8651-D6C10378128C}"/>
-    <hyperlink ref="B2" r:id="rId24" xr:uid="{DE5B31BF-642F-4D65-BB0B-8BB02C0C599F}"/>
-    <hyperlink ref="B123" r:id="rId25" xr:uid="{6478F936-7CCC-485F-8FAD-5E974D281F62}"/>
-    <hyperlink ref="B96" r:id="rId26" xr:uid="{4FDE78C3-89C9-4179-86C1-21A106ED4B68}"/>
-    <hyperlink ref="B75" r:id="rId27" xr:uid="{71FF812A-69FD-42EC-A428-9503EB1166BE}"/>
-    <hyperlink ref="B144" r:id="rId28" xr:uid="{6A269B70-A168-4F22-809C-69E3664B7B4F}"/>
-    <hyperlink ref="B80" r:id="rId29" xr:uid="{2AF8C5A2-0A6E-4AFA-BE5A-8756CD3E9A15}"/>
-    <hyperlink ref="B106" r:id="rId30" xr:uid="{775807C5-A8E8-4E03-94A3-07FC338C7B2F}"/>
-    <hyperlink ref="B146" r:id="rId31" xr:uid="{4C620958-7BE1-4A72-AF05-2D2C30EFE637}"/>
-    <hyperlink ref="B111" r:id="rId32" xr:uid="{9C374395-032E-47D8-8E1D-F14135FEB884}"/>
-    <hyperlink ref="B6" r:id="rId33" xr:uid="{7C24BFBA-D940-4280-9AA6-9EB5B2A7C325}"/>
-    <hyperlink ref="B11" r:id="rId34" xr:uid="{935A4BCA-043C-42B5-9B58-F01D785A78E7}"/>
-    <hyperlink ref="B132" r:id="rId35" xr:uid="{AD23B2E5-01B6-4980-8B3E-2745128B55B6}"/>
-    <hyperlink ref="B95" r:id="rId36" xr:uid="{ADD15800-FFAF-4C56-96C3-B6E9A6B7A9B4}"/>
-    <hyperlink ref="B54" r:id="rId37" xr:uid="{FD14EBC0-A744-44D9-8D7E-8C400674FEED}"/>
-    <hyperlink ref="B24" r:id="rId38" xr:uid="{1C789BBB-C806-4AEC-87FD-4A30D09E0378}"/>
-    <hyperlink ref="B94" r:id="rId39" xr:uid="{39BDDF5C-5ED6-4DC6-8403-935839E42AE4}"/>
-    <hyperlink ref="B131" r:id="rId40" xr:uid="{16CEFA6F-1B35-42FD-8606-E6523BF824B9}"/>
-    <hyperlink ref="B62:B78" r:id="rId41" display="https://midfield.mlbstatic.com/v1/people/686752/spots/120" xr:uid="{1E5EFC44-7608-40AF-A777-AAC898C6A9CB}"/>
-    <hyperlink ref="B21" r:id="rId42" xr:uid="{17D051F0-8C68-4AF3-B256-1F5E71DD2455}"/>
-    <hyperlink ref="B56" r:id="rId43" xr:uid="{B4766B4E-7BF7-4C41-98C2-8E48C0CCFAC8}"/>
-    <hyperlink ref="B69" r:id="rId44" xr:uid="{49ACB698-CD82-44AA-8A65-26D2BBDB0788}"/>
-    <hyperlink ref="B41" r:id="rId45" xr:uid="{FBAE3FE6-1362-4C09-BAE7-1B131AB4C4B4}"/>
-    <hyperlink ref="B36" r:id="rId46" xr:uid="{2181E8B2-59C9-4709-AA9A-962EF37831F2}"/>
-    <hyperlink ref="B67" r:id="rId47" xr:uid="{17F5505C-32E7-4316-BF97-1E84202C4785}"/>
-    <hyperlink ref="B50" r:id="rId48" xr:uid="{880E4723-2052-4A3F-AA76-423C6810C994}"/>
-    <hyperlink ref="B101" r:id="rId49" xr:uid="{D33AE6C2-8688-4E9D-B293-9E99FBE0DEB4}"/>
-    <hyperlink ref="B49" r:id="rId50" xr:uid="{ECF4F8FF-BB1E-4B49-965D-64768DC4F1E2}"/>
-    <hyperlink ref="B63" r:id="rId51" xr:uid="{2511CD2C-B67C-4354-9629-DE649A920EDD}"/>
-    <hyperlink ref="B138" r:id="rId52" xr:uid="{AE0C1E2C-3D72-45CF-9965-CDB6C0591891}"/>
-    <hyperlink ref="B64" r:id="rId53" xr:uid="{0E258565-BD6E-428A-BCE6-5D446B3DA628}"/>
-    <hyperlink ref="B43" r:id="rId54" xr:uid="{46541DDA-A399-42E9-B388-CAC462670117}"/>
-    <hyperlink ref="B112" r:id="rId55" xr:uid="{E26B4D45-A378-40C0-ACBA-A3D7F3B56528}"/>
-    <hyperlink ref="B100" r:id="rId56" xr:uid="{845F84C0-232D-4D80-B9DD-7415056297C5}"/>
-    <hyperlink ref="B133" r:id="rId57" xr:uid="{89BF64D4-12AC-4144-8B32-FDDD10668077}"/>
-    <hyperlink ref="B102" r:id="rId58" xr:uid="{8742B9B5-62C4-423F-B53B-AE1C619A7CB3}"/>
-    <hyperlink ref="B60" r:id="rId59" xr:uid="{A93F2FF5-2AE8-404E-A935-39A2AA8E0351}"/>
-    <hyperlink ref="B91" r:id="rId60" xr:uid="{F60D4181-1F3A-4C64-97A2-8368BC1A6176}"/>
-    <hyperlink ref="B142" r:id="rId61" xr:uid="{ECDB48F3-3C25-4B15-A902-40A90B1D441F}"/>
-    <hyperlink ref="B98" r:id="rId62" xr:uid="{1BF5B84A-6403-496F-BE72-4F7CFE5CD46A}"/>
-    <hyperlink ref="B58" r:id="rId63" xr:uid="{D48CC097-21D9-4697-92AF-17FE888C3469}"/>
-    <hyperlink ref="B153" r:id="rId64" xr:uid="{BA111F30-72E9-4701-B810-D904333C5C12}"/>
-    <hyperlink ref="B109" r:id="rId65" xr:uid="{C971DFEC-7D7D-44F8-8D77-AF06DD0C3650}"/>
-    <hyperlink ref="B157" r:id="rId66" xr:uid="{FF747A90-D82C-417A-A604-11C8A9BB8A1B}"/>
-    <hyperlink ref="B78" r:id="rId67" xr:uid="{508F6AEF-0519-456E-95D4-CFBA12F1D839}"/>
-    <hyperlink ref="B92" r:id="rId68" xr:uid="{B67845F2-3B4F-45CB-AC96-C32761C20607}"/>
-    <hyperlink ref="B137" r:id="rId69" xr:uid="{B3EDDFE1-3BCD-4BF4-B469-F8CBF05D5228}"/>
-    <hyperlink ref="B22" r:id="rId70" xr:uid="{8E3867C0-9128-44B4-8D0A-62F663FD1C50}"/>
-    <hyperlink ref="B34" r:id="rId71" xr:uid="{7DF45689-E876-4814-B27F-BD82DF1893A8}"/>
-    <hyperlink ref="B134" r:id="rId72" xr:uid="{10233510-1E7F-47D8-9DC8-CECCEEAF2542}"/>
-    <hyperlink ref="B84" r:id="rId73" xr:uid="{C4B8637F-0EAC-421C-B98A-83396BEC74E6}"/>
-    <hyperlink ref="B7" r:id="rId74" xr:uid="{78FBD904-905A-4DF4-8336-339D9FD35EF9}"/>
-    <hyperlink ref="B155" r:id="rId75" xr:uid="{30FFC8B8-F48B-4956-82E5-5F5C1D42BFDA}"/>
-    <hyperlink ref="B127" r:id="rId76" xr:uid="{F297C688-6767-4A01-87CA-713F0DDF9C34}"/>
-    <hyperlink ref="B32" r:id="rId77" xr:uid="{DE8C1BDA-4F06-4739-8272-9C1526634215}"/>
-    <hyperlink ref="B150" r:id="rId78" xr:uid="{0B5DD545-15F8-4AED-86A6-780BA78A0233}"/>
-    <hyperlink ref="B81" r:id="rId79" xr:uid="{1EAB83F2-BCC3-4788-AB88-9206EE59BEFD}"/>
-    <hyperlink ref="B89" r:id="rId80" xr:uid="{B9CEB789-AD16-4793-B005-DBCE618DBE94}"/>
-    <hyperlink ref="B159" r:id="rId81" xr:uid="{BE0D192A-BC2F-4B35-99E0-370F38CA9C0B}"/>
-    <hyperlink ref="B48" r:id="rId82" xr:uid="{3F8FC17C-F146-4E12-BBB9-18B45BB5B3EC}"/>
-    <hyperlink ref="B72" r:id="rId83" xr:uid="{C3C3E0D1-E6BE-417A-AC79-EEB8F79FBE7C}"/>
-    <hyperlink ref="B39" r:id="rId84" xr:uid="{646B995D-2022-47E8-9C46-F74E16A3A629}"/>
-    <hyperlink ref="B37" r:id="rId85" xr:uid="{1F133298-7E48-4138-8126-F74D2CBDB050}"/>
-    <hyperlink ref="B149" r:id="rId86" xr:uid="{79CA2660-030A-4E38-B36D-D5A391C24AF6}"/>
-    <hyperlink ref="B105" r:id="rId87" xr:uid="{301BF770-273A-484E-AF66-F32DA8458844}"/>
-    <hyperlink ref="B160" r:id="rId88" xr:uid="{A72F7411-3596-45A9-BD47-96AE1238FE57}"/>
-    <hyperlink ref="B79" r:id="rId89" xr:uid="{9335E23F-5F7C-4364-8ABA-564F1B156EB5}"/>
-    <hyperlink ref="B93" r:id="rId90" xr:uid="{C528D45E-5270-4308-A5F4-DDDD4C29A97D}"/>
-    <hyperlink ref="B83" r:id="rId91" xr:uid="{E5C83DAC-00EF-49EE-9811-99C544403146}"/>
-    <hyperlink ref="B125" r:id="rId92" xr:uid="{F5146A50-BA2B-4466-A3AC-A9E6870FA443}"/>
-    <hyperlink ref="B121" r:id="rId93" xr:uid="{880D6AB9-DCD2-4819-B973-72461A04C7C8}"/>
-    <hyperlink ref="B136" r:id="rId94" xr:uid="{11544622-27D7-41FE-BA8C-7A64E8838D48}"/>
-    <hyperlink ref="B35" r:id="rId95" xr:uid="{BC65DFE4-1308-4C08-8CE7-8941756F790F}"/>
-    <hyperlink ref="B73" r:id="rId96" xr:uid="{8322B7F1-705E-4313-8FF2-F90CCF591E35}"/>
-    <hyperlink ref="B108" r:id="rId97" xr:uid="{EBB28F68-D663-44AA-86BD-53B20904935E}"/>
-    <hyperlink ref="B85" r:id="rId98" xr:uid="{6A80E6A8-DBFE-4A55-A512-7374F8FBE4FD}"/>
-    <hyperlink ref="B40" r:id="rId99" xr:uid="{CE6A856C-5BA0-46B8-BDBB-70D03B1E5FA6}"/>
-    <hyperlink ref="B44" r:id="rId100" xr:uid="{B219EA6C-AFC6-4A8E-A965-70B93C5367C4}"/>
-    <hyperlink ref="B156" r:id="rId101" xr:uid="{108B5805-5369-47C0-A3A2-CA30D2F91CFB}"/>
-    <hyperlink ref="B76" r:id="rId102" xr:uid="{7AD71135-DE45-46BB-A218-39306ABA3702}"/>
-    <hyperlink ref="B107:B115" r:id="rId103" display="https://midfield.mlbstatic.com/v1/people/570632/spots/120" xr:uid="{B6AEF0A1-DAD3-493D-AD72-9992AF4AC36A}"/>
-    <hyperlink ref="B139" r:id="rId104" xr:uid="{4FC1EEA6-0897-4ECD-9CE7-1A38B7A04DF4}"/>
-    <hyperlink ref="B115" r:id="rId105" xr:uid="{1C2C51A3-E75B-4CC0-A087-8366DF24A3F2}"/>
-    <hyperlink ref="B128" r:id="rId106" xr:uid="{BB7DF76E-86EB-4858-AEA6-0696B62895BC}"/>
-    <hyperlink ref="B14" r:id="rId107" xr:uid="{01DE55D4-78E8-461B-A8B9-B03E6D65C918}"/>
-    <hyperlink ref="B46" r:id="rId108" xr:uid="{FCD4C620-BB71-4CC3-A123-50EFE98B5FE2}"/>
-    <hyperlink ref="B124" r:id="rId109" xr:uid="{29ED6610-0117-47A3-9540-69CB5AC80B92}"/>
-    <hyperlink ref="B140" r:id="rId110" xr:uid="{9E30FD12-A196-40BE-A210-0C73986E5064}"/>
-    <hyperlink ref="B147" r:id="rId111" xr:uid="{B8175F43-D70E-459F-98CF-15ECFA717548}"/>
-    <hyperlink ref="B90" r:id="rId112" xr:uid="{A1F217DD-45E3-4ABD-A801-5D9F166E4EE3}"/>
-    <hyperlink ref="B10" r:id="rId113" xr:uid="{C6E8A0D7-8E63-4EC1-8C28-4570F13EECF8}"/>
-    <hyperlink ref="B26" r:id="rId114" xr:uid="{061EEF2C-85CF-400C-B70C-3AC1B107F1EC}"/>
-    <hyperlink ref="B27" r:id="rId115" xr:uid="{07D08D3B-A3C3-4916-9FE0-2CF26ECA4304}"/>
-    <hyperlink ref="B47" r:id="rId116" xr:uid="{91E7913A-86EE-40F5-9798-4A7B25F420CA}"/>
-    <hyperlink ref="B87" r:id="rId117" xr:uid="{0A5A0FD7-8B57-41D3-A410-CA8F6779F8C0}"/>
-    <hyperlink ref="B103" r:id="rId118" xr:uid="{9979CA0C-3483-428F-A7AC-8624936FB8FA}"/>
-    <hyperlink ref="B118" r:id="rId119" xr:uid="{482918C2-89BA-496F-8160-085C2940475B}"/>
-    <hyperlink ref="B122" r:id="rId120" xr:uid="{674942CB-83E4-4508-A135-1EB5B6D6E0BF}"/>
-    <hyperlink ref="B145" r:id="rId121" xr:uid="{1F6209AE-91BF-41D4-B9AD-7DEABA16621B}"/>
-    <hyperlink ref="B148" r:id="rId122" xr:uid="{F0E5D36A-2456-4111-9B29-31D8CBD1A12D}"/>
-    <hyperlink ref="B154" r:id="rId123" xr:uid="{789C651E-21E8-4E0D-8017-9BF6770B7FE4}"/>
-    <hyperlink ref="B143" r:id="rId124" xr:uid="{E96CD394-E5F8-46F9-9A93-3EA98A4EE8DE}"/>
-    <hyperlink ref="B16" r:id="rId125" xr:uid="{170B8200-FCC5-4ED1-8A6A-63B3F60FC427}"/>
-    <hyperlink ref="B19" r:id="rId126" xr:uid="{1165D173-E61C-477D-81EA-53C274E42084}"/>
-    <hyperlink ref="B8" r:id="rId127" xr:uid="{D71E6989-E12D-4FB6-8277-45C3718AA5C4}"/>
-    <hyperlink ref="B5" r:id="rId128" xr:uid="{FB4F273B-2196-4018-85BA-D42A207F8910}"/>
-    <hyperlink ref="B62" r:id="rId129" xr:uid="{9F233235-B9B1-4E7A-807E-8F2EE493E173}"/>
-    <hyperlink ref="B126" r:id="rId130" xr:uid="{F5D1A66D-4324-4468-A7A0-AD3D00B16AE7}"/>
-    <hyperlink ref="B18" r:id="rId131" xr:uid="{1759929B-600A-4949-96E1-F424E054D97A}"/>
-    <hyperlink ref="B86" r:id="rId132" xr:uid="{8B19E95A-E327-406E-9F25-861358533D76}"/>
-    <hyperlink ref="B17" r:id="rId133" xr:uid="{1DD3FDF5-6556-4823-8827-A75B5E83FD01}"/>
-    <hyperlink ref="B152" r:id="rId134" xr:uid="{B62475DC-179F-4CE0-8CF6-51DC972D40B7}"/>
-    <hyperlink ref="B151" r:id="rId135" xr:uid="{492088BD-9B89-42AA-A6AF-1F83749BDC72}"/>
-    <hyperlink ref="B20" r:id="rId136" xr:uid="{6118D192-2DB6-4311-A382-3371906C183D}"/>
-    <hyperlink ref="B140:B143" r:id="rId137" display="https://midfield.mlbstatic.com/v1/people/693821/spots/120" xr:uid="{0E83A794-B683-4463-A3A3-95576AFDD615}"/>
-    <hyperlink ref="B38" r:id="rId138" xr:uid="{98EC2002-988D-46D0-AD8B-CB1135815ADD}"/>
-    <hyperlink ref="B161" r:id="rId139" xr:uid="{80C5B6A6-E3F5-4F34-8C17-B202CF8842F5}"/>
-    <hyperlink ref="B113" r:id="rId140" xr:uid="{35842AC4-F920-4A32-B105-587FE352F876}"/>
-    <hyperlink ref="B68" r:id="rId141" xr:uid="{24E2A301-E80D-4F02-A94B-CFE6DF3719D1}"/>
-    <hyperlink ref="B59" r:id="rId142" xr:uid="{6D687EFE-5BD7-4FEF-B636-1A728E3CB6DF}"/>
-    <hyperlink ref="B119" r:id="rId143" xr:uid="{20E003D8-D5C4-4113-AFC3-D076CE9FE0A0}"/>
-    <hyperlink ref="B99" r:id="rId144" xr:uid="{3D5F262E-120A-4E2A-AF3A-1C4C1117AE44}"/>
-    <hyperlink ref="B15" r:id="rId145" xr:uid="{5ED77DE1-166F-4541-898A-786E114DAEF4}"/>
-    <hyperlink ref="B25" r:id="rId146" xr:uid="{81DC0D20-42F6-4D3C-87D3-B645CB35712A}"/>
-    <hyperlink ref="B30" r:id="rId147" xr:uid="{E396E594-A4D8-4E20-9A24-90B7589370B5}"/>
-    <hyperlink ref="B51" r:id="rId148" xr:uid="{823E8EED-4901-4993-A8EA-2CA91EBD8526}"/>
-    <hyperlink ref="B61" r:id="rId149" xr:uid="{923E21E9-8410-4112-9000-9E93896189E6}"/>
-    <hyperlink ref="B88" r:id="rId150" xr:uid="{C526E886-242E-4E87-ACB6-1E69A02EEBD3}"/>
-    <hyperlink ref="B104" r:id="rId151" xr:uid="{BFEEE380-0C63-474F-821D-61F8EF908A46}"/>
-    <hyperlink ref="B114" r:id="rId152" xr:uid="{2250FC95-0A39-4EE2-BCB2-FFF1EF3E4964}"/>
-    <hyperlink ref="B77" r:id="rId153" xr:uid="{174AA7F5-75DB-42B1-ACFF-646023A4BD2A}"/>
-    <hyperlink ref="B141" r:id="rId154" xr:uid="{30D34D43-AD29-4DE6-93CC-FD7C2F05FE00}"/>
-    <hyperlink ref="B110" r:id="rId155" xr:uid="{AD2496AE-C6CA-4D48-BE1B-E0D40292B961}"/>
-    <hyperlink ref="B82" r:id="rId156" xr:uid="{8EA8AFE5-38A5-4C45-95E6-52202880E214}"/>
-    <hyperlink ref="B107" r:id="rId157" xr:uid="{933DFE08-9AFA-4E05-81A6-D7AD9B2936B4}"/>
-    <hyperlink ref="B130" r:id="rId158" xr:uid="{5CB1E923-0C0B-46C3-9A06-C5BF1664BB99}"/>
-    <hyperlink ref="B4" r:id="rId159" xr:uid="{F0633C7D-B030-42F8-867D-487A4D0622C9}"/>
-    <hyperlink ref="B13" r:id="rId160" xr:uid="{F7C050ED-4E17-4083-9409-29763900B9F8}"/>
-    <hyperlink ref="B53" r:id="rId161" xr:uid="{96DF98C5-93EB-4B46-A8DE-540F97FB9D2D}"/>
-    <hyperlink ref="B163" r:id="rId162" xr:uid="{DC3780E6-8DBB-43AF-868F-038344C91A4E}"/>
-    <hyperlink ref="B164" r:id="rId163" xr:uid="{AF843F30-7625-42D0-BA56-6434FAE62C25}"/>
-    <hyperlink ref="B165" r:id="rId164" xr:uid="{5D94729E-5BC9-4A90-91A4-E22E6DF54EC5}"/>
-    <hyperlink ref="B166" r:id="rId165" xr:uid="{07FE2158-E54F-4DAF-A552-7A5F3BB2BAF7}"/>
-    <hyperlink ref="B29" r:id="rId166" xr:uid="{202CCF33-99A3-4853-AE16-95008489CCC5}"/>
-    <hyperlink ref="B42" r:id="rId167" xr:uid="{F4B5E23D-9319-41A2-AB51-5DE0A45DD8B4}"/>
-    <hyperlink ref="B71" r:id="rId168" xr:uid="{1692F5E0-FB63-492A-92F7-244666AA4D6C}"/>
-    <hyperlink ref="B167" r:id="rId169" xr:uid="{AB038426-E25A-4D00-959B-BADAAFC83263}"/>
-    <hyperlink ref="B168" r:id="rId170" xr:uid="{37BD58F8-5963-4DEE-8AC0-94C476AAA7B4}"/>
-    <hyperlink ref="B169" r:id="rId171" xr:uid="{224B22F8-17AF-4F0E-B83D-83E51925E3DA}"/>
-    <hyperlink ref="B170" r:id="rId172" xr:uid="{7C41A3D8-7B2C-4E19-8D41-28A0650CBF55}"/>
-    <hyperlink ref="B171" r:id="rId173" xr:uid="{04763326-6E4F-46B3-85EC-C59D9071D0F0}"/>
-    <hyperlink ref="B172" r:id="rId174" xr:uid="{6595AC92-4EB6-4C25-8AA6-B1D9744B1285}"/>
-    <hyperlink ref="B173" r:id="rId175" xr:uid="{B78F9174-E83B-47E6-946E-143B1E2D43D8}"/>
-    <hyperlink ref="B174" r:id="rId176" xr:uid="{063DB121-1B09-4C4A-A7CB-67F92A70E822}"/>
-    <hyperlink ref="B175" r:id="rId177" xr:uid="{4529126A-013E-48BE-BF9C-0857DD382C6C}"/>
-    <hyperlink ref="B176" r:id="rId178" xr:uid="{2F41BBD7-2015-4D42-8F88-8932B17FA34E}"/>
-    <hyperlink ref="B177" r:id="rId179" xr:uid="{E3EEE818-F47C-4DA4-97C5-449CA4C17CE4}"/>
-    <hyperlink ref="B178" r:id="rId180" xr:uid="{9F68A673-C7E6-4A90-BBDE-1C7409208E96}"/>
-    <hyperlink ref="B179" r:id="rId181" xr:uid="{889380E0-647D-4489-BE9B-25BAE5EB7861}"/>
-    <hyperlink ref="B180" r:id="rId182" xr:uid="{E541544B-61E3-4737-BBE7-E7662EC00A72}"/>
-    <hyperlink ref="B181" r:id="rId183" xr:uid="{4BE71305-E922-40EC-A901-A899B6397770}"/>
-    <hyperlink ref="B182" r:id="rId184" xr:uid="{1DB36123-F811-448C-80B1-68D23463FD4D}"/>
-    <hyperlink ref="B183" r:id="rId185" xr:uid="{3C679776-3AB8-453B-A4D3-B37792A73D16}"/>
-    <hyperlink ref="B184" r:id="rId186" xr:uid="{FA711ADD-C082-40DD-82D1-0E78DD912F0F}"/>
-    <hyperlink ref="B185" r:id="rId187" xr:uid="{C7B04CD8-F035-43DB-A418-9133A48E8921}"/>
-    <hyperlink ref="B186" r:id="rId188" xr:uid="{53F20A14-3749-4B51-B405-0EB1EA8BE457}"/>
-    <hyperlink ref="B187" r:id="rId189" xr:uid="{F2A8C005-E73E-4EA8-9A69-7D1C21C8DA9F}"/>
-    <hyperlink ref="B188" r:id="rId190" xr:uid="{E1A325DE-861E-4917-B535-A3626E67093B}"/>
-    <hyperlink ref="B189" r:id="rId191" xr:uid="{0B8721CA-ADDC-484A-A593-AA5D129028A4}"/>
-    <hyperlink ref="B190" r:id="rId192" xr:uid="{976908EE-A22D-40EC-95CA-B678C03D5727}"/>
-    <hyperlink ref="B191" r:id="rId193" xr:uid="{2359E283-699E-4E88-A140-3D7A568FC6E6}"/>
-    <hyperlink ref="B192" r:id="rId194" xr:uid="{6EAF58AD-5C21-4CAF-9E5B-779352704AB8}"/>
-    <hyperlink ref="B193" r:id="rId195" xr:uid="{075C6DD4-9B5F-454C-9441-F8AB51EBBED6}"/>
-    <hyperlink ref="B194" r:id="rId196" xr:uid="{2AB02CE7-6DE6-4936-A9B6-C3A30517DB7F}"/>
-    <hyperlink ref="B195" r:id="rId197" xr:uid="{3FA450BF-3E01-439C-8C3C-97285CDF42E4}"/>
-    <hyperlink ref="B196" r:id="rId198" xr:uid="{B7C88999-8CA0-468E-9DB7-0C84FECCE62D}"/>
-    <hyperlink ref="B197" r:id="rId199" xr:uid="{4030FD80-AC58-4604-AAD9-3C8DDF33D9BF}"/>
-    <hyperlink ref="B198" r:id="rId200" xr:uid="{A6D3B7B5-05D6-404A-A466-9DFEDA40D0C8}"/>
-    <hyperlink ref="B199" r:id="rId201" xr:uid="{E49A6EE8-5822-4020-9BE9-083EAD5C84FB}"/>
-    <hyperlink ref="B200" r:id="rId202" xr:uid="{9CB2615F-20AF-4560-8DE8-06A6D01F94D3}"/>
-    <hyperlink ref="B201" r:id="rId203" xr:uid="{050FB622-EB1C-4B7B-9B5C-D0165F6DB2BB}"/>
+    <hyperlink ref="C135" r:id="rId1" xr:uid="{C45472D7-1E29-4980-95E0-15D6D01B36FA}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{1EA6B6DE-C528-4BBF-8958-B9D1378CBBEA}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{4F9BBF32-0E85-44F1-BAE2-FDFE1B91203C}"/>
+    <hyperlink ref="C28" r:id="rId4" xr:uid="{1743C8BA-2A45-4EF9-8EAE-003FA5622677}"/>
+    <hyperlink ref="C120" r:id="rId5" xr:uid="{759148E7-8E0F-41F6-B9F3-BB34C434E2D7}"/>
+    <hyperlink ref="C129" r:id="rId6" xr:uid="{8850343C-EAF0-4713-9C66-21BF05B290EC}"/>
+    <hyperlink ref="C31" r:id="rId7" xr:uid="{CA8DDB4C-49CE-4AA5-B564-1108A8088B23}"/>
+    <hyperlink ref="C45" r:id="rId8" xr:uid="{A96A63DD-6ED4-47E6-B759-BD9FCFC58B60}"/>
+    <hyperlink ref="C162" r:id="rId9" xr:uid="{55C307B9-C21E-4227-B6BA-602B4CDD2E63}"/>
+    <hyperlink ref="C117" r:id="rId10" xr:uid="{FBC71765-97DF-4951-8AED-C771FFA6C3B6}"/>
+    <hyperlink ref="C52" r:id="rId11" xr:uid="{44C0BA97-BC98-4009-9EF5-8C29C471CC2B}"/>
+    <hyperlink ref="C65" r:id="rId12" xr:uid="{83CC39A1-58DF-4F8E-80EF-7133BFDA09E5}"/>
+    <hyperlink ref="C66" r:id="rId13" xr:uid="{A9F4C6E5-7612-40C3-92FF-2F0A1197F32E}"/>
+    <hyperlink ref="C55" r:id="rId14" xr:uid="{29AD0F25-0604-4645-86CB-591ACB87642C}"/>
+    <hyperlink ref="C33" r:id="rId15" xr:uid="{03239B77-EAD5-4377-8E99-41BDC8C35FAF}"/>
+    <hyperlink ref="C57" r:id="rId16" xr:uid="{A963AD17-9953-4B76-B014-99AE04AFBC22}"/>
+    <hyperlink ref="C23" r:id="rId17" xr:uid="{254FC5D9-2139-49F1-AF42-C37C7AD52CF9}"/>
+    <hyperlink ref="C97" r:id="rId18" xr:uid="{ADEC84CE-4B4C-475A-B45C-A5A25ABA57F9}"/>
+    <hyperlink ref="C70" r:id="rId19" xr:uid="{A903E050-8C42-4183-880A-565DF6E20245}"/>
+    <hyperlink ref="C3" r:id="rId20" xr:uid="{E83EAE86-523E-449E-8625-E0FCBC6EDE67}"/>
+    <hyperlink ref="C158" r:id="rId21" xr:uid="{4F43B789-DA90-4D7B-B4C4-7719C98AFEF4}"/>
+    <hyperlink ref="C116" r:id="rId22" xr:uid="{1073D5D0-0D5E-4AB1-940D-24EDB5EF0E1D}"/>
+    <hyperlink ref="C74" r:id="rId23" xr:uid="{30F225A0-9236-482B-8651-D6C10378128C}"/>
+    <hyperlink ref="C2" r:id="rId24" xr:uid="{DE5B31BF-642F-4D65-BB0B-8BB02C0C599F}"/>
+    <hyperlink ref="C123" r:id="rId25" xr:uid="{6478F936-7CCC-485F-8FAD-5E974D281F62}"/>
+    <hyperlink ref="C96" r:id="rId26" xr:uid="{4FDE78C3-89C9-4179-86C1-21A106ED4B68}"/>
+    <hyperlink ref="C75" r:id="rId27" xr:uid="{71FF812A-69FD-42EC-A428-9503EB1166BE}"/>
+    <hyperlink ref="C144" r:id="rId28" xr:uid="{6A269B70-A168-4F22-809C-69E3664B7B4F}"/>
+    <hyperlink ref="C80" r:id="rId29" xr:uid="{2AF8C5A2-0A6E-4AFA-BE5A-8756CD3E9A15}"/>
+    <hyperlink ref="C106" r:id="rId30" xr:uid="{775807C5-A8E8-4E03-94A3-07FC338C7B2F}"/>
+    <hyperlink ref="C146" r:id="rId31" xr:uid="{4C620958-7BE1-4A72-AF05-2D2C30EFE637}"/>
+    <hyperlink ref="C111" r:id="rId32" xr:uid="{9C374395-032E-47D8-8E1D-F14135FEB884}"/>
+    <hyperlink ref="C6" r:id="rId33" xr:uid="{7C24BFBA-D940-4280-9AA6-9EB5B2A7C325}"/>
+    <hyperlink ref="C11" r:id="rId34" xr:uid="{935A4BCA-043C-42B5-9B58-F01D785A78E7}"/>
+    <hyperlink ref="C132" r:id="rId35" xr:uid="{AD23B2E5-01B6-4980-8B3E-2745128B55B6}"/>
+    <hyperlink ref="C95" r:id="rId36" xr:uid="{ADD15800-FFAF-4C56-96C3-B6E9A6B7A9B4}"/>
+    <hyperlink ref="C54" r:id="rId37" xr:uid="{FD14EBC0-A744-44D9-8D7E-8C400674FEED}"/>
+    <hyperlink ref="C24" r:id="rId38" xr:uid="{1C789BBB-C806-4AEC-87FD-4A30D09E0378}"/>
+    <hyperlink ref="C94" r:id="rId39" xr:uid="{39BDDF5C-5ED6-4DC6-8403-935839E42AE4}"/>
+    <hyperlink ref="C131" r:id="rId40" xr:uid="{16CEFA6F-1B35-42FD-8606-E6523BF824B9}"/>
+    <hyperlink ref="C62:C78" r:id="rId41" display="https://midfield.mlbstatic.com/v1/people/686752/spots/120" xr:uid="{1E5EFC44-7608-40AF-A777-AAC898C6A9CB}"/>
+    <hyperlink ref="C21" r:id="rId42" xr:uid="{17D051F0-8C68-4AF3-B256-1F5E71DD2455}"/>
+    <hyperlink ref="C56" r:id="rId43" xr:uid="{B4766B4E-7BF7-4C41-98C2-8E48C0CCFAC8}"/>
+    <hyperlink ref="C69" r:id="rId44" xr:uid="{49ACB698-CD82-44AA-8A65-26D2BBDB0788}"/>
+    <hyperlink ref="C41" r:id="rId45" xr:uid="{FBAE3FE6-1362-4C09-BAE7-1B131AB4C4B4}"/>
+    <hyperlink ref="C36" r:id="rId46" xr:uid="{2181E8B2-59C9-4709-AA9A-962EF37831F2}"/>
+    <hyperlink ref="C67" r:id="rId47" xr:uid="{17F5505C-32E7-4316-BF97-1E84202C4785}"/>
+    <hyperlink ref="C50" r:id="rId48" xr:uid="{880E4723-2052-4A3F-AA76-423C6810C994}"/>
+    <hyperlink ref="C101" r:id="rId49" xr:uid="{D33AE6C2-8688-4E9D-B293-9E99FBE0DEB4}"/>
+    <hyperlink ref="C49" r:id="rId50" xr:uid="{ECF4F8FF-BB1E-4B49-965D-64768DC4F1E2}"/>
+    <hyperlink ref="C63" r:id="rId51" xr:uid="{2511CD2C-B67C-4354-9629-DE649A920EDD}"/>
+    <hyperlink ref="C138" r:id="rId52" xr:uid="{AE0C1E2C-3D72-45CF-9965-CDB6C0591891}"/>
+    <hyperlink ref="C64" r:id="rId53" xr:uid="{0E258565-BD6E-428A-BCE6-5D446B3DA628}"/>
+    <hyperlink ref="C43" r:id="rId54" xr:uid="{46541DDA-A399-42E9-B388-CAC462670117}"/>
+    <hyperlink ref="C112" r:id="rId55" xr:uid="{E26B4D45-A378-40C0-ACBA-A3D7F3B56528}"/>
+    <hyperlink ref="C100" r:id="rId56" xr:uid="{845F84C0-232D-4D80-B9DD-7415056297C5}"/>
+    <hyperlink ref="C133" r:id="rId57" xr:uid="{89BF64D4-12AC-4144-8B32-FDDD10668077}"/>
+    <hyperlink ref="C102" r:id="rId58" xr:uid="{8742B9B5-62C4-423F-B53B-AE1C619A7CB3}"/>
+    <hyperlink ref="C60" r:id="rId59" xr:uid="{A93F2FF5-2AE8-404E-A935-39A2AA8E0351}"/>
+    <hyperlink ref="C91" r:id="rId60" xr:uid="{F60D4181-1F3A-4C64-97A2-8368BC1A6176}"/>
+    <hyperlink ref="C142" r:id="rId61" xr:uid="{ECDB48F3-3C25-4B15-A902-40A90B1D441F}"/>
+    <hyperlink ref="C98" r:id="rId62" xr:uid="{1BF5B84A-6403-496F-BE72-4F7CFE5CD46A}"/>
+    <hyperlink ref="C58" r:id="rId63" xr:uid="{D48CC097-21D9-4697-92AF-17FE888C3469}"/>
+    <hyperlink ref="C153" r:id="rId64" xr:uid="{BA111F30-72E9-4701-B810-D904333C5C12}"/>
+    <hyperlink ref="C109" r:id="rId65" xr:uid="{C971DFEC-7D7D-44F8-8D77-AF06DD0C3650}"/>
+    <hyperlink ref="C157" r:id="rId66" xr:uid="{FF747A90-D82C-417A-A604-11C8A9BB8A1B}"/>
+    <hyperlink ref="C78" r:id="rId67" xr:uid="{508F6AEF-0519-456E-95D4-CFBA12F1D839}"/>
+    <hyperlink ref="C92" r:id="rId68" xr:uid="{B67845F2-3B4F-45CB-AC96-C32761C20607}"/>
+    <hyperlink ref="C137" r:id="rId69" xr:uid="{B3EDDFE1-3BCD-4BF4-B469-F8CBF05D5228}"/>
+    <hyperlink ref="C22" r:id="rId70" xr:uid="{8E3867C0-9128-44B4-8D0A-62F663FD1C50}"/>
+    <hyperlink ref="C34" r:id="rId71" xr:uid="{7DF45689-E876-4814-B27F-BD82DF1893A8}"/>
+    <hyperlink ref="C134" r:id="rId72" xr:uid="{10233510-1E7F-47D8-9DC8-CECCEEAF2542}"/>
+    <hyperlink ref="C84" r:id="rId73" xr:uid="{C4B8637F-0EAC-421C-B98A-83396BEC74E6}"/>
+    <hyperlink ref="C7" r:id="rId74" xr:uid="{78FBD904-905A-4DF4-8336-339D9FD35EF9}"/>
+    <hyperlink ref="C155" r:id="rId75" xr:uid="{30FFC8B8-F48B-4956-82E5-5F5C1D42BFDA}"/>
+    <hyperlink ref="C127" r:id="rId76" xr:uid="{F297C688-6767-4A01-87CA-713F0DDF9C34}"/>
+    <hyperlink ref="C32" r:id="rId77" xr:uid="{DE8C1BDA-4F06-4739-8272-9C1526634215}"/>
+    <hyperlink ref="C150" r:id="rId78" xr:uid="{0B5DD545-15F8-4AED-86A6-780BA78A0233}"/>
+    <hyperlink ref="C81" r:id="rId79" xr:uid="{1EAB83F2-BCC3-4788-AB88-9206EE59BEFD}"/>
+    <hyperlink ref="C89" r:id="rId80" xr:uid="{B9CEB789-AD16-4793-B005-DBCE618DBE94}"/>
+    <hyperlink ref="C159" r:id="rId81" xr:uid="{BE0D192A-BC2F-4B35-99E0-370F38CA9C0B}"/>
+    <hyperlink ref="C48" r:id="rId82" xr:uid="{3F8FC17C-F146-4E12-BBB9-18B45BB5B3EC}"/>
+    <hyperlink ref="C72" r:id="rId83" xr:uid="{C3C3E0D1-E6BE-417A-AC79-EEB8F79FBE7C}"/>
+    <hyperlink ref="C39" r:id="rId84" xr:uid="{646B995D-2022-47E8-9C46-F74E16A3A629}"/>
+    <hyperlink ref="C37" r:id="rId85" xr:uid="{1F133298-7E48-4138-8126-F74D2CBDB050}"/>
+    <hyperlink ref="C149" r:id="rId86" xr:uid="{79CA2660-030A-4E38-B36D-D5A391C24AF6}"/>
+    <hyperlink ref="C105" r:id="rId87" xr:uid="{301BF770-273A-484E-AF66-F32DA8458844}"/>
+    <hyperlink ref="C160" r:id="rId88" xr:uid="{A72F7411-3596-45A9-BD47-96AE1238FE57}"/>
+    <hyperlink ref="C79" r:id="rId89" xr:uid="{9335E23F-5F7C-4364-8ABA-564F1B156EB5}"/>
+    <hyperlink ref="C93" r:id="rId90" xr:uid="{C528D45E-5270-4308-A5F4-DDDD4C29A97D}"/>
+    <hyperlink ref="C83" r:id="rId91" xr:uid="{E5C83DAC-00EF-49EE-9811-99C544403146}"/>
+    <hyperlink ref="C125" r:id="rId92" xr:uid="{F5146A50-BA2B-4466-A3AC-A9E6870FA443}"/>
+    <hyperlink ref="C121" r:id="rId93" xr:uid="{880D6AB9-DCD2-4819-B973-72461A04C7C8}"/>
+    <hyperlink ref="C136" r:id="rId94" xr:uid="{11544622-27D7-41FE-BA8C-7A64E8838D48}"/>
+    <hyperlink ref="C35" r:id="rId95" xr:uid="{BC65DFE4-1308-4C08-8CE7-8941756F790F}"/>
+    <hyperlink ref="C73" r:id="rId96" xr:uid="{8322B7F1-705E-4313-8FF2-F90CCF591E35}"/>
+    <hyperlink ref="C108" r:id="rId97" xr:uid="{EBB28F68-D663-44AA-86BD-53B20904935E}"/>
+    <hyperlink ref="C85" r:id="rId98" xr:uid="{6A80E6A8-DBFE-4A55-A512-7374F8FBE4FD}"/>
+    <hyperlink ref="C40" r:id="rId99" xr:uid="{CE6A856C-5BA0-46B8-BDBB-70D03B1E5FA6}"/>
+    <hyperlink ref="C44" r:id="rId100" xr:uid="{B219EA6C-AFC6-4A8E-A965-70B93C5367C4}"/>
+    <hyperlink ref="C156" r:id="rId101" xr:uid="{108B5805-5369-47C0-A3A2-CA30D2F91CFB}"/>
+    <hyperlink ref="C76" r:id="rId102" xr:uid="{7AD71135-DE45-46BB-A218-39306ABA3702}"/>
+    <hyperlink ref="C107:C115" r:id="rId103" display="https://midfield.mlbstatic.com/v1/people/570632/spots/120" xr:uid="{B6AEF0A1-DAD3-493D-AD72-9992AF4AC36A}"/>
+    <hyperlink ref="C139" r:id="rId104" xr:uid="{4FC1EEA6-0897-4ECD-9CE7-1A38B7A04DF4}"/>
+    <hyperlink ref="C115" r:id="rId105" xr:uid="{1C2C51A3-E75B-4CC0-A087-8366DF24A3F2}"/>
+    <hyperlink ref="C128" r:id="rId106" xr:uid="{BB7DF76E-86EB-4858-AEA6-0696B62895BC}"/>
+    <hyperlink ref="C14" r:id="rId107" xr:uid="{01DE55D4-78E8-461B-A8B9-B03E6D65C918}"/>
+    <hyperlink ref="C46" r:id="rId108" xr:uid="{FCD4C620-BB71-4CC3-A123-50EFE98B5FE2}"/>
+    <hyperlink ref="C124" r:id="rId109" xr:uid="{29ED6610-0117-47A3-9540-69CB5AC80B92}"/>
+    <hyperlink ref="C140" r:id="rId110" xr:uid="{9E30FD12-A196-40BE-A210-0C73986E5064}"/>
+    <hyperlink ref="C147" r:id="rId111" xr:uid="{B8175F43-D70E-459F-98CF-15ECFA717548}"/>
+    <hyperlink ref="C90" r:id="rId112" xr:uid="{A1F217DD-45E3-4ABD-A801-5D9F166E4EE3}"/>
+    <hyperlink ref="C10" r:id="rId113" xr:uid="{C6E8A0D7-8E63-4EC1-8C28-4570F13EECF8}"/>
+    <hyperlink ref="C26" r:id="rId114" xr:uid="{061EEF2C-85CF-400C-B70C-3AC1B107F1EC}"/>
+    <hyperlink ref="C27" r:id="rId115" xr:uid="{07D08D3B-A3C3-4916-9FE0-2CF26ECA4304}"/>
+    <hyperlink ref="C47" r:id="rId116" xr:uid="{91E7913A-86EE-40F5-9798-4A7B25F420CA}"/>
+    <hyperlink ref="C87" r:id="rId117" xr:uid="{0A5A0FD7-8B57-41D3-A410-CA8F6779F8C0}"/>
+    <hyperlink ref="C103" r:id="rId118" xr:uid="{9979CA0C-3483-428F-A7AC-8624936FB8FA}"/>
+    <hyperlink ref="C118" r:id="rId119" xr:uid="{482918C2-89BA-496F-8160-085C2940475B}"/>
+    <hyperlink ref="C122" r:id="rId120" xr:uid="{674942CB-83E4-4508-A135-1EB5B6D6E0BF}"/>
+    <hyperlink ref="C145" r:id="rId121" xr:uid="{1F6209AE-91BF-41D4-B9AD-7DEABA16621B}"/>
+    <hyperlink ref="C148" r:id="rId122" xr:uid="{F0E5D36A-2456-4111-9B29-31D8CBD1A12D}"/>
+    <hyperlink ref="C154" r:id="rId123" xr:uid="{789C651E-21E8-4E0D-8017-9BF6770B7FE4}"/>
+    <hyperlink ref="C143" r:id="rId124" xr:uid="{E96CD394-E5F8-46F9-9A93-3EA98A4EE8DE}"/>
+    <hyperlink ref="C16" r:id="rId125" xr:uid="{170B8200-FCC5-4ED1-8A6A-63B3F60FC427}"/>
+    <hyperlink ref="C19" r:id="rId126" xr:uid="{1165D173-E61C-477D-81EA-53C274E42084}"/>
+    <hyperlink ref="C8" r:id="rId127" xr:uid="{D71E6989-E12D-4FB6-8277-45C3718AA5C4}"/>
+    <hyperlink ref="C5" r:id="rId128" xr:uid="{FB4F273B-2196-4018-85BA-D42A207F8910}"/>
+    <hyperlink ref="C62" r:id="rId129" xr:uid="{9F233235-B9B1-4E7A-807E-8F2EE493E173}"/>
+    <hyperlink ref="C126" r:id="rId130" xr:uid="{F5D1A66D-4324-4468-A7A0-AD3D00B16AE7}"/>
+    <hyperlink ref="C18" r:id="rId131" xr:uid="{1759929B-600A-4949-96E1-F424E054D97A}"/>
+    <hyperlink ref="C86" r:id="rId132" xr:uid="{8B19E95A-E327-406E-9F25-861358533D76}"/>
+    <hyperlink ref="C17" r:id="rId133" xr:uid="{1DD3FDF5-6556-4823-8827-A75B5E83FD01}"/>
+    <hyperlink ref="C152" r:id="rId134" xr:uid="{B62475DC-179F-4CE0-8CF6-51DC972D40B7}"/>
+    <hyperlink ref="C151" r:id="rId135" xr:uid="{492088BD-9B89-42AA-A6AF-1F83749BDC72}"/>
+    <hyperlink ref="C20" r:id="rId136" xr:uid="{6118D192-2DB6-4311-A382-3371906C183D}"/>
+    <hyperlink ref="C140:C143" r:id="rId137" display="https://midfield.mlbstatic.com/v1/people/693821/spots/120" xr:uid="{0E83A794-B683-4463-A3A3-95576AFDD615}"/>
+    <hyperlink ref="C38" r:id="rId138" xr:uid="{98EC2002-988D-46D0-AD8B-CB1135815ADD}"/>
+    <hyperlink ref="C161" r:id="rId139" xr:uid="{80C5B6A6-E3F5-4F34-8C17-B202CF8842F5}"/>
+    <hyperlink ref="C113" r:id="rId140" xr:uid="{35842AC4-F920-4A32-B105-587FE352F876}"/>
+    <hyperlink ref="C68" r:id="rId141" xr:uid="{24E2A301-E80D-4F02-A94B-CFE6DF3719D1}"/>
+    <hyperlink ref="C59" r:id="rId142" xr:uid="{6D687EFE-5BD7-4FEF-B636-1A728E3CB6DF}"/>
+    <hyperlink ref="C119" r:id="rId143" xr:uid="{20E003D8-D5C4-4113-AFC3-D076CE9FE0A0}"/>
+    <hyperlink ref="C99" r:id="rId144" xr:uid="{3D5F262E-120A-4E2A-AF3A-1C4C1117AE44}"/>
+    <hyperlink ref="C15" r:id="rId145" xr:uid="{5ED77DE1-166F-4541-898A-786E114DAEF4}"/>
+    <hyperlink ref="C25" r:id="rId146" xr:uid="{81DC0D20-42F6-4D3C-87D3-B645CB35712A}"/>
+    <hyperlink ref="C30" r:id="rId147" xr:uid="{E396E594-A4D8-4E20-9A24-90B7589370B5}"/>
+    <hyperlink ref="C51" r:id="rId148" xr:uid="{823E8EED-4901-4993-A8EA-2CA91EBD8526}"/>
+    <hyperlink ref="C61" r:id="rId149" xr:uid="{923E21E9-8410-4112-9000-9E93896189E6}"/>
+    <hyperlink ref="C88" r:id="rId150" xr:uid="{C526E886-242E-4E87-ACB6-1E69A02EEBD3}"/>
+    <hyperlink ref="C104" r:id="rId151" xr:uid="{BFEEE380-0C63-474F-821D-61F8EF908A46}"/>
+    <hyperlink ref="C114" r:id="rId152" xr:uid="{2250FC95-0A39-4EE2-BCB2-FFF1EF3E4964}"/>
+    <hyperlink ref="C77" r:id="rId153" xr:uid="{174AA7F5-75DB-42B1-ACFF-646023A4BD2A}"/>
+    <hyperlink ref="C141" r:id="rId154" xr:uid="{30D34D43-AD29-4DE6-93CC-FD7C2F05FE00}"/>
+    <hyperlink ref="C110" r:id="rId155" xr:uid="{AD2496AE-C6CA-4D48-BE1B-E0D40292B961}"/>
+    <hyperlink ref="C82" r:id="rId156" xr:uid="{8EA8AFE5-38A5-4C45-95E6-52202880E214}"/>
+    <hyperlink ref="C107" r:id="rId157" xr:uid="{933DFE08-9AFA-4E05-81A6-D7AD9B2936B4}"/>
+    <hyperlink ref="C130" r:id="rId158" xr:uid="{5CB1E923-0C0B-46C3-9A06-C5BF1664BB99}"/>
+    <hyperlink ref="C4" r:id="rId159" xr:uid="{F0633C7D-B030-42F8-867D-487A4D0622C9}"/>
+    <hyperlink ref="C13" r:id="rId160" xr:uid="{F7C050ED-4E17-4083-9409-29763900B9F8}"/>
+    <hyperlink ref="C53" r:id="rId161" xr:uid="{96DF98C5-93EB-4B46-A8DE-540F97FB9D2D}"/>
+    <hyperlink ref="C163" r:id="rId162" xr:uid="{DC3780E6-8DBB-43AF-868F-038344C91A4E}"/>
+    <hyperlink ref="C164" r:id="rId163" xr:uid="{AF843F30-7625-42D0-BA56-6434FAE62C25}"/>
+    <hyperlink ref="C165" r:id="rId164" xr:uid="{5D94729E-5BC9-4A90-91A4-E22E6DF54EC5}"/>
+    <hyperlink ref="C166" r:id="rId165" xr:uid="{07FE2158-E54F-4DAF-A552-7A5F3BB2BAF7}"/>
+    <hyperlink ref="C29" r:id="rId166" xr:uid="{202CCF33-99A3-4853-AE16-95008489CCC5}"/>
+    <hyperlink ref="C42" r:id="rId167" xr:uid="{F4B5E23D-9319-41A2-AB51-5DE0A45DD8B4}"/>
+    <hyperlink ref="C71" r:id="rId168" xr:uid="{1692F5E0-FB63-492A-92F7-244666AA4D6C}"/>
+    <hyperlink ref="C167" r:id="rId169" xr:uid="{AB038426-E25A-4D00-959B-BADAAFC83263}"/>
+    <hyperlink ref="C168" r:id="rId170" xr:uid="{37BD58F8-5963-4DEE-8AC0-94C476AAA7B4}"/>
+    <hyperlink ref="C169" r:id="rId171" xr:uid="{224B22F8-17AF-4F0E-B83D-83E51925E3DA}"/>
+    <hyperlink ref="C170" r:id="rId172" xr:uid="{7C41A3D8-7B2C-4E19-8D41-28A0650CBF55}"/>
+    <hyperlink ref="C171" r:id="rId173" xr:uid="{04763326-6E4F-46B3-85EC-C59D9071D0F0}"/>
+    <hyperlink ref="C172" r:id="rId174" xr:uid="{6595AC92-4EB6-4C25-8AA6-B1D9744B1285}"/>
+    <hyperlink ref="C173" r:id="rId175" xr:uid="{B78F9174-E83B-47E6-946E-143B1E2D43D8}"/>
+    <hyperlink ref="C174" r:id="rId176" xr:uid="{063DB121-1B09-4C4A-A7CB-67F92A70E822}"/>
+    <hyperlink ref="C175" r:id="rId177" xr:uid="{4529126A-013E-48BE-BF9C-0857DD382C6C}"/>
+    <hyperlink ref="C176" r:id="rId178" xr:uid="{2F41BBD7-2015-4D42-8F88-8932B17FA34E}"/>
+    <hyperlink ref="C177" r:id="rId179" xr:uid="{E3EEE818-F47C-4DA4-97C5-449CA4C17CE4}"/>
+    <hyperlink ref="C178" r:id="rId180" xr:uid="{9F68A673-C7E6-4A90-BBDE-1C7409208E96}"/>
+    <hyperlink ref="C179" r:id="rId181" xr:uid="{889380E0-647D-4489-BE9B-25BAE5EB7861}"/>
+    <hyperlink ref="C180" r:id="rId182" xr:uid="{E541544B-61E3-4737-BBE7-E7662EC00A72}"/>
+    <hyperlink ref="C181" r:id="rId183" xr:uid="{4BE71305-E922-40EC-A901-A899B6397770}"/>
+    <hyperlink ref="C182" r:id="rId184" xr:uid="{1DB36123-F811-448C-80B1-68D23463FD4D}"/>
+    <hyperlink ref="C183" r:id="rId185" xr:uid="{3C679776-3AB8-453B-A4D3-B37792A73D16}"/>
+    <hyperlink ref="C184" r:id="rId186" xr:uid="{FA711ADD-C082-40DD-82D1-0E78DD912F0F}"/>
+    <hyperlink ref="C185" r:id="rId187" xr:uid="{C7B04CD8-F035-43DB-A418-9133A48E8921}"/>
+    <hyperlink ref="C186" r:id="rId188" xr:uid="{53F20A14-3749-4B51-B405-0EB1EA8BE457}"/>
+    <hyperlink ref="C187" r:id="rId189" xr:uid="{F2A8C005-E73E-4EA8-9A69-7D1C21C8DA9F}"/>
+    <hyperlink ref="C188" r:id="rId190" xr:uid="{E1A325DE-861E-4917-B535-A3626E67093B}"/>
+    <hyperlink ref="C189" r:id="rId191" xr:uid="{0B8721CA-ADDC-484A-A593-AA5D129028A4}"/>
+    <hyperlink ref="C190" r:id="rId192" xr:uid="{976908EE-A22D-40EC-95CA-B678C03D5727}"/>
+    <hyperlink ref="C191" r:id="rId193" xr:uid="{2359E283-699E-4E88-A140-3D7A568FC6E6}"/>
+    <hyperlink ref="C192" r:id="rId194" xr:uid="{6EAF58AD-5C21-4CAF-9E5B-779352704AB8}"/>
+    <hyperlink ref="C193" r:id="rId195" xr:uid="{075C6DD4-9B5F-454C-9441-F8AB51EBBED6}"/>
+    <hyperlink ref="C194" r:id="rId196" xr:uid="{2AB02CE7-6DE6-4936-A9B6-C3A30517DB7F}"/>
+    <hyperlink ref="C195" r:id="rId197" xr:uid="{3FA450BF-3E01-439C-8C3C-97285CDF42E4}"/>
+    <hyperlink ref="C196" r:id="rId198" xr:uid="{B7C88999-8CA0-468E-9DB7-0C84FECCE62D}"/>
+    <hyperlink ref="C197" r:id="rId199" xr:uid="{4030FD80-AC58-4604-AAD9-3C8DDF33D9BF}"/>
+    <hyperlink ref="C198" r:id="rId200" xr:uid="{A6D3B7B5-05D6-404A-A466-9DFEDA40D0C8}"/>
+    <hyperlink ref="C199" r:id="rId201" xr:uid="{E49A6EE8-5822-4020-9BE9-083EAD5C84FB}"/>
+    <hyperlink ref="C200" r:id="rId202" xr:uid="{9CB2615F-20AF-4560-8DE8-06A6D01F94D3}"/>
+    <hyperlink ref="C201" r:id="rId203" xr:uid="{050FB622-EB1C-4B7B-9B5C-D0165F6DB2BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
trying to fix player names
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79695CCE-603F-48A7-90F8-4C9E2FD32370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D39AAD-F28D-4C42-A93D-A594A42BE621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4459,11 +4459,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D162">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C135" r:id="rId1" xr:uid="{C45472D7-1E29-4980-95E0-15D6D01B36FA}"/>
     <hyperlink ref="C9" r:id="rId2" xr:uid="{1EA6B6DE-C528-4BBF-8958-B9D1378CBBEA}"/>

</xml_diff>

<commit_message>
Pushing June 11 files
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D39AAD-F28D-4C42-A93D-A594A42BE621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880E74F5-C9DC-4B7A-AFA7-B01064007C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="408">
   <si>
     <t>Name</t>
   </si>
@@ -1242,6 +1242,27 @@
   </si>
   <si>
     <t>Baseball_Savant_Name</t>
+  </si>
+  <si>
+    <t>Drew Thorpe</t>
+  </si>
+  <si>
+    <t>Jose Suarez</t>
+  </si>
+  <si>
+    <t>Louie Varland</t>
+  </si>
+  <si>
+    <t>Carlos Rodriguez</t>
+  </si>
+  <si>
+    <t>José Suarez</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/660761/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/686973/spots/120</t>
   </si>
 </sst>
 </file>
@@ -1631,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4456,6 +4477,59 @@
       </c>
       <c r="D201" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>401</v>
+      </c>
+      <c r="B202" t="s">
+        <v>401</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D202" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>402</v>
+      </c>
+      <c r="B203" t="s">
+        <v>405</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D203" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>403</v>
+      </c>
+      <c r="B204" t="s">
+        <v>403</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D204" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>404</v>
+      </c>
+      <c r="B205" t="s">
+        <v>404</v>
+      </c>
+      <c r="D205" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4663,6 +4737,9 @@
     <hyperlink ref="C199" r:id="rId201" xr:uid="{E49A6EE8-5822-4020-9BE9-083EAD5C84FB}"/>
     <hyperlink ref="C200" r:id="rId202" xr:uid="{9CB2615F-20AF-4560-8DE8-06A6D01F94D3}"/>
     <hyperlink ref="C201" r:id="rId203" xr:uid="{050FB622-EB1C-4B7B-9B5C-D0165F6DB2BB}"/>
+    <hyperlink ref="C202" r:id="rId204" xr:uid="{B0AA3E5E-F474-4547-A4BB-1562AFD05639}"/>
+    <hyperlink ref="C203" r:id="rId205" xr:uid="{5EE48E44-6645-423B-9D3B-BA27E3C88CF6}"/>
+    <hyperlink ref="C204" r:id="rId206" xr:uid="{DC2CCDEC-A6B0-4412-9293-3D708FF0E861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating June 15 file
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1362A30-626A-4C07-A805-796BCBC3D339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FDBF06-CE81-47E1-B294-66A651038CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8208" yWindow="1704" windowWidth="17280" windowHeight="8880" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="418">
   <si>
     <t>Name</t>
   </si>
@@ -1287,6 +1287,12 @@
   </si>
   <si>
     <t>Roddery Muñoz</t>
+  </si>
+  <si>
+    <t>Tommy Henry</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/674072/spots/120</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D210" sqref="D210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4598,6 +4604,20 @@
         <v>414</v>
       </c>
       <c r="D208" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" t="s">
+        <v>416</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D209" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4813,7 +4833,9 @@
     <hyperlink ref="C207" r:id="rId208" xr:uid="{4423E675-229D-4F9B-9CC0-F8C46E201512}"/>
     <hyperlink ref="C205" r:id="rId209" xr:uid="{4DA93860-D7DA-4B52-A9A0-ABAC3B793A26}"/>
     <hyperlink ref="C208" r:id="rId210" xr:uid="{FA66E72F-4556-483C-AED4-B7C4E5F6ED33}"/>
+    <hyperlink ref="C209" r:id="rId211" xr:uid="{6B606037-8FCB-4B89-85F6-9C109BB639E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId212"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating pitchers and stats
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FDBF06-CE81-47E1-B294-66A651038CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FB8C31-A6B4-4055-AB3A-8AAA4969B778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="423">
   <si>
     <t>Name</t>
   </si>
@@ -1133,9 +1133,6 @@
     <t>https://midfield.mlbstatic.com/v1/people/547001/spots/120</t>
   </si>
   <si>
-    <t>Tyler Megill</t>
-  </si>
-  <si>
     <t>https://midfield.mlbstatic.com/v1/people/656731/spots/120</t>
   </si>
   <si>
@@ -1293,6 +1290,24 @@
   </si>
   <si>
     <t>https://midfield.mlbstatic.com/v1/people/674072/spots/120</t>
+  </si>
+  <si>
+    <t>Jesús Luzardo</t>
+  </si>
+  <si>
+    <t>Josh Fleming</t>
+  </si>
+  <si>
+    <t>Tylor Megill</t>
+  </si>
+  <si>
+    <t>Spencer Bivens</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/676595/spots/120</t>
+  </si>
+  <si>
+    <t>https://midfield.mlbstatic.com/v1/people/702352/spots/120</t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2033,10 +2048,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>288</v>
@@ -3464,7 +3479,7 @@
         <v>35</v>
       </c>
       <c r="B127" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>170</v>
@@ -4273,13 +4288,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>419</v>
+      </c>
+      <c r="B185" t="s">
+        <v>419</v>
+      </c>
+      <c r="C185" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="B185" t="s">
-        <v>364</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="D185" t="s">
         <v>164</v>
@@ -4287,13 +4302,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B186" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D186" t="s">
         <v>164</v>
@@ -4301,13 +4316,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B187" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D187" t="s">
         <v>164</v>
@@ -4315,13 +4330,13 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B188" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D188" t="s">
         <v>164</v>
@@ -4329,13 +4344,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B189" t="s">
-        <v>371</v>
+        <v>417</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D189" t="s">
         <v>161</v>
@@ -4343,13 +4358,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B190" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D190" t="s">
         <v>161</v>
@@ -4357,13 +4372,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B191" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D191" t="s">
         <v>164</v>
@@ -4371,13 +4386,13 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>377</v>
+      </c>
+      <c r="B192" t="s">
+        <v>377</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B192" t="s">
-        <v>378</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="D192" t="s">
         <v>161</v>
@@ -4385,13 +4400,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B193" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D193" t="s">
         <v>164</v>
@@ -4399,13 +4414,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B194" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D194" t="s">
         <v>161</v>
@@ -4413,13 +4428,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>383</v>
+      </c>
+      <c r="B195" t="s">
+        <v>383</v>
+      </c>
+      <c r="C195" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B195" t="s">
-        <v>384</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="D195" t="s">
         <v>161</v>
@@ -4427,13 +4442,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B196" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D196" t="s">
         <v>164</v>
@@ -4441,13 +4456,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>386</v>
+      </c>
+      <c r="B197" t="s">
+        <v>386</v>
+      </c>
+      <c r="C197" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B197" t="s">
-        <v>387</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="D197" t="s">
         <v>164</v>
@@ -4455,13 +4470,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B198" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D198" t="s">
         <v>164</v>
@@ -4469,13 +4484,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>389</v>
+      </c>
+      <c r="B199" t="s">
+        <v>389</v>
+      </c>
+      <c r="C199" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B199" t="s">
-        <v>390</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="D199" t="s">
         <v>164</v>
@@ -4483,13 +4498,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B200" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D200" t="s">
         <v>164</v>
@@ -4497,13 +4512,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B201" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D201" t="s">
         <v>161</v>
@@ -4511,13 +4526,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B202" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D202" t="s">
         <v>164</v>
@@ -4525,13 +4540,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B203" t="s">
+        <v>404</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="D203" t="s">
         <v>161</v>
@@ -4539,13 +4554,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B204" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D204" t="s">
         <v>164</v>
@@ -4553,13 +4568,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B205" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D205" t="s">
         <v>164</v>
@@ -4567,13 +4582,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>407</v>
+      </c>
+      <c r="B206" t="s">
+        <v>407</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="B206" t="s">
-        <v>408</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="D206" t="s">
         <v>161</v>
@@ -4581,13 +4596,13 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>409</v>
+      </c>
+      <c r="B207" t="s">
+        <v>409</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="B207" t="s">
-        <v>410</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="D207" t="s">
         <v>164</v>
@@ -4595,13 +4610,13 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>412</v>
+      </c>
+      <c r="B208" t="s">
+        <v>412</v>
+      </c>
+      <c r="C208" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="B208" t="s">
-        <v>413</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>414</v>
       </c>
       <c r="D208" t="s">
         <v>161</v>
@@ -4609,16 +4624,44 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>415</v>
+      </c>
+      <c r="B209" t="s">
+        <v>415</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B209" t="s">
-        <v>416</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="D209" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" t="s">
+        <v>418</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D210" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" t="s">
+        <v>420</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D211" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4834,8 +4877,10 @@
     <hyperlink ref="C205" r:id="rId209" xr:uid="{4DA93860-D7DA-4B52-A9A0-ABAC3B793A26}"/>
     <hyperlink ref="C208" r:id="rId210" xr:uid="{FA66E72F-4556-483C-AED4-B7C4E5F6ED33}"/>
     <hyperlink ref="C209" r:id="rId211" xr:uid="{6B606037-8FCB-4B89-85F6-9C109BB639E4}"/>
+    <hyperlink ref="C210" r:id="rId212" xr:uid="{043B1326-06A0-4BFB-AE2B-D08C2362D448}"/>
+    <hyperlink ref="C211" r:id="rId213" xr:uid="{ED67AC35-5992-4B66-83D1-089BA4E99A16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId212"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId214"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update pitcher headshots file
</commit_message>
<xml_diff>
--- a/assets/Pitcher_Headshots.xlsx
+++ b/assets/Pitcher_Headshots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB959108-6856-4100-B6DA-B51FE7AE6868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8D5B10-5B6B-4A5A-AD57-4955B7C2E015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485955CB-CA9F-4484-BF64-3C0860480D03}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="434">
   <si>
     <t>Name</t>
   </si>
@@ -1338,6 +1338,9 @@
   </si>
   <si>
     <t>https://midfield.mlbstatic.com/v1/people/543037/spots/120</t>
+  </si>
+  <si>
+    <t>Ranger Suárez</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8121A6F-EAC3-49EE-8365-3E22E9EB309E}">
   <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="D216" sqref="D216"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3439,7 +3442,7 @@
         <v>239</v>
       </c>
       <c r="B122" t="s">
-        <v>239</v>
+        <v>433</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>240</v>

</xml_diff>